<commit_message>
partie 2 + tableau complété
</commit_message>
<xml_diff>
--- a/testchi2utile.xlsx
+++ b/testchi2utile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Desktop\ENSAI\Projet_Stat\projetstat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C08653-BC15-4135-831C-E91E8494D7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAA529E-F838-4641-AB41-A0738D8D5A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CA859BD4-508A-4149-A9AE-557F09B1B32B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>mise_habituelle</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Medecin</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4A48C4-AD14-492C-BCF6-7C70F2E86EF4}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,6 +892,58 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>16.838999999999999</v>
+      </c>
+      <c r="D17">
+        <v>4.8149999999999998E-3</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>9.5639000000000003</v>
+      </c>
+      <c r="D18">
+        <v>8.8580000000000006E-2</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>